<commit_message>
MainTEMPs - Updated Rock Lobster Landings Template ...
</commit_message>
<xml_diff>
--- a/Landings/LANDINGS_Rock_Lobster_(Jasus_lalandii).xlsx
+++ b/Landings/LANDINGS_Rock_Lobster_(Jasus_lalandii).xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="909"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="909" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="00. META-Rights" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="140">
   <si>
     <t>Index</t>
   </si>
@@ -418,13 +418,49 @@
   </si>
   <si>
     <t>Owner Contact (Mobile)</t>
+  </si>
+  <si>
+    <t>-&gt; The Seasonal "Landings" Data for the Namibian Spiny Rock Lobster (SRL) Commercial Fishing Sector …</t>
+  </si>
+  <si>
+    <t>-&gt; The Seasonal "Quota Allocation" Data …</t>
+  </si>
+  <si>
+    <t>Season:</t>
+  </si>
+  <si>
+    <t>LANDED SOUTH</t>
+  </si>
+  <si>
+    <t>LANDED NORTH</t>
+  </si>
+  <si>
+    <t>CENTRAL</t>
+  </si>
+  <si>
+    <t>F/NORTH</t>
+  </si>
+  <si>
+    <t>TOTAL LANDED</t>
+  </si>
+  <si>
+    <t>REMAINING DIFFERENCE</t>
+  </si>
+  <si>
+    <t>STATUS</t>
+  </si>
+  <si>
+    <t>EXCEEDED QUOTA</t>
+  </si>
+  <si>
+    <t>QUOTA ALLOCATED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -467,8 +503,21 @@
       <name val="Cambria"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF0000CC"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0000CC"/>
+      <name val="Cambria"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -478,6 +527,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,7 +555,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -508,9 +569,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -530,6 +588,20 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,14 +737,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="49.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="20.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="25" style="1" customWidth="1"/>
     <col min="5" max="5" width="35" style="1" customWidth="1"/>
@@ -681,59 +753,59 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
     </row>
     <row r="2" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="17" t="s">
         <v>40</v>
       </c>
       <c r="G2" s="3"/>
       <c r="H2" s="3"/>
     </row>
     <row r="3" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -744,7 +816,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -755,7 +827,7 @@
       </c>
     </row>
     <row r="5" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
@@ -766,7 +838,7 @@
       </c>
     </row>
     <row r="6" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="16">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -774,7 +846,7 @@
       </c>
     </row>
     <row r="7" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="16">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
@@ -782,7 +854,7 @@
       </c>
     </row>
     <row r="8" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="16">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
@@ -793,7 +865,7 @@
       </c>
     </row>
     <row r="9" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="16">
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
@@ -801,7 +873,7 @@
       </c>
     </row>
     <row r="10" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="16">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
@@ -809,7 +881,7 @@
       </c>
     </row>
     <row r="11" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="16">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
@@ -817,7 +889,7 @@
       </c>
     </row>
     <row r="12" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="16">
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
@@ -825,7 +897,7 @@
       </c>
     </row>
     <row r="13" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="16">
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -833,7 +905,7 @@
       </c>
     </row>
     <row r="14" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="16">
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
@@ -844,7 +916,7 @@
       </c>
     </row>
     <row r="15" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="16">
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
@@ -852,7 +924,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="16">
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
@@ -860,7 +932,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="16">
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -868,7 +940,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="16">
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
@@ -876,7 +948,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19" s="16">
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
@@ -884,7 +956,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="16">
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
@@ -892,7 +964,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="16">
         <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
@@ -900,7 +972,7 @@
       </c>
     </row>
     <row r="22" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="16">
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
@@ -908,7 +980,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="16">
         <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
@@ -916,7 +988,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="16">
         <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
@@ -924,7 +996,7 @@
       </c>
     </row>
     <row r="25" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="16">
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
@@ -932,7 +1004,7 @@
       </c>
     </row>
     <row r="26" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26" s="16">
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
@@ -940,7 +1012,7 @@
       </c>
     </row>
     <row r="27" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="A27" s="16">
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
@@ -948,7 +1020,7 @@
       </c>
     </row>
     <row r="28" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+      <c r="A28" s="16">
         <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
@@ -956,7 +1028,7 @@
       </c>
     </row>
     <row r="29" spans="1:2" s="4" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+      <c r="A29" s="16">
         <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
@@ -964,7 +1036,7 @@
       </c>
     </row>
     <row r="30" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="A30" s="16">
         <v>28</v>
       </c>
       <c r="B30" s="5" t="s">
@@ -972,7 +1044,7 @@
       </c>
     </row>
     <row r="31" spans="1:2" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="A31" s="16">
         <v>29</v>
       </c>
       <c r="B31" s="5" t="s">
@@ -1027,559 +1099,559 @@
   <dimension ref="A1:Z32"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="17.85546875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="33.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.42578125" style="12" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.85546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.28515625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="11.5703125" style="12"/>
+    <col min="1" max="1" width="7.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="17.85546875" style="12" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.85546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.28515625" style="11" bestFit="1" customWidth="1"/>
+    <col min="10" max="16384" width="11.5703125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="4" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="11"/>
-      <c r="X1" s="11"/>
-      <c r="Y1" s="11"/>
-      <c r="Z1" s="11"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F2" s="16" t="s">
         <v>123</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="18" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>99</v>
       </c>
       <c r="E3" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F3" s="7">
+      <c r="F3" s="6">
         <v>14.77</v>
       </c>
-      <c r="G3" s="7">
+      <c r="G3" s="6">
         <v>1980</v>
       </c>
       <c r="H3" s="4"/>
     </row>
     <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>100</v>
       </c>
       <c r="E4" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F4" s="7"/>
-      <c r="G4" s="7">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6">
         <v>1981</v>
       </c>
       <c r="H4" s="4"/>
     </row>
     <row r="5" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>101</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7">
+      <c r="F5" s="6"/>
+      <c r="G5" s="6">
         <v>1984</v>
       </c>
       <c r="H5" s="4"/>
     </row>
     <row r="6" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+      <c r="A6" s="16">
         <v>4</v>
       </c>
       <c r="B6" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>102</v>
       </c>
       <c r="E6" s="4"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
       <c r="H6" s="4"/>
     </row>
     <row r="7" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+      <c r="A7" s="16">
         <v>5</v>
       </c>
       <c r="B7" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="7" t="s">
+      <c r="C7" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="6" t="s">
         <v>103</v>
       </c>
       <c r="E7" s="4"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
       <c r="H7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+      <c r="A8" s="16">
         <v>6</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>104</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
       <c r="H8" s="4"/>
     </row>
     <row r="9" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+      <c r="A9" s="16">
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D9" s="6" t="s">
         <v>105</v>
       </c>
       <c r="E9" s="4"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="7"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
       <c r="H9" s="4"/>
     </row>
     <row r="10" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+      <c r="A10" s="16">
         <v>8</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="6" t="s">
         <v>106</v>
       </c>
       <c r="E10" s="4"/>
-      <c r="F10" s="7"/>
-      <c r="G10" s="7"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
       <c r="H10" s="4"/>
     </row>
     <row r="11" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+      <c r="A11" s="16">
         <v>9</v>
       </c>
       <c r="B11" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C11" s="7" t="s">
+      <c r="C11" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="D11" s="6" t="s">
         <v>107</v>
       </c>
       <c r="E11" s="4"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
       <c r="H11" s="4"/>
     </row>
     <row r="12" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+      <c r="A12" s="16">
         <v>10</v>
       </c>
       <c r="B12" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="7" t="s">
+      <c r="C12" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="D12" s="6" t="s">
         <v>108</v>
       </c>
       <c r="E12" s="4"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="7"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
       <c r="H12" s="4"/>
     </row>
     <row r="13" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+      <c r="A13" s="16">
         <v>11</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="7" t="s">
+      <c r="C13" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="D13" s="7" t="s">
+      <c r="D13" s="6" t="s">
         <v>109</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="F13" s="7"/>
-      <c r="G13" s="7">
+      <c r="F13" s="6"/>
+      <c r="G13" s="6">
         <v>1985</v>
       </c>
       <c r="H13" s="4"/>
     </row>
     <row r="14" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+      <c r="A14" s="16">
         <v>12</v>
       </c>
       <c r="B14" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="7" t="s">
+      <c r="C14" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="D14" s="7" t="s">
+      <c r="D14" s="6" t="s">
         <v>110</v>
       </c>
       <c r="E14" s="4"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
       <c r="H14" s="4"/>
     </row>
     <row r="15" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+      <c r="A15" s="16">
         <v>13</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="C15" s="7" t="s">
+      <c r="C15" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="D15" s="6" t="s">
         <v>111</v>
       </c>
       <c r="E15" s="4"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
       <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+      <c r="A16" s="16">
         <v>14</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="C16" s="7" t="s">
+      <c r="C16" s="6" t="s">
         <v>89</v>
       </c>
-      <c r="D16" s="7" t="s">
+      <c r="D16" s="6" t="s">
         <v>112</v>
       </c>
       <c r="E16" s="4"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
       <c r="H16" s="4"/>
     </row>
     <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+      <c r="A17" s="16">
         <v>15</v>
       </c>
       <c r="B17" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="7" t="s">
+      <c r="C17" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="7" t="s">
+      <c r="D17" s="6" t="s">
         <v>113</v>
       </c>
       <c r="E17" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F17" s="7">
+      <c r="F17" s="6">
         <v>3.5</v>
       </c>
-      <c r="G17" s="7"/>
+      <c r="G17" s="6"/>
       <c r="H17" s="4"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+      <c r="A18" s="16">
         <v>16</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="7" t="s">
+      <c r="C18" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="D18" s="7" t="s">
+      <c r="D18" s="6" t="s">
         <v>114</v>
       </c>
       <c r="E18" s="4"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
       <c r="H18" s="4"/>
     </row>
     <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+      <c r="A19" s="16">
         <v>17</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="7" t="s">
+      <c r="C19" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="D19" s="6" t="s">
         <v>98</v>
       </c>
       <c r="E19" s="4"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
       <c r="H19" s="4"/>
     </row>
     <row r="20" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+      <c r="A20" s="16">
         <v>18</v>
       </c>
       <c r="B20" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C20" s="7" t="s">
+      <c r="C20" s="6" t="s">
         <v>93</v>
       </c>
-      <c r="D20" s="7" t="s">
+      <c r="D20" s="6" t="s">
         <v>115</v>
       </c>
       <c r="E20" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="F20" s="7">
+      <c r="F20" s="6">
         <v>14.75</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>125</v>
       </c>
       <c r="H20" s="4"/>
     </row>
     <row r="21" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+      <c r="A21" s="16">
         <v>19</v>
       </c>
       <c r="B21" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="C21" s="7" t="s">
+      <c r="C21" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="7" t="s">
+      <c r="D21" s="6" t="s">
         <v>116</v>
       </c>
       <c r="E21" s="4"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="7"/>
+      <c r="F21" s="6"/>
+      <c r="G21" s="6"/>
       <c r="H21" s="4"/>
     </row>
     <row r="22" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+      <c r="A22" s="16">
         <v>20</v>
       </c>
       <c r="B22" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>117</v>
       </c>
       <c r="E22" s="4"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
       <c r="H22" s="4"/>
     </row>
     <row r="23" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+      <c r="A23" s="16">
         <v>21</v>
       </c>
       <c r="B23" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C23" s="7" t="s">
+      <c r="C23" s="6" t="s">
         <v>96</v>
       </c>
-      <c r="D23" s="7" t="s">
+      <c r="D23" s="6" t="s">
         <v>118</v>
       </c>
       <c r="E23" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F23" s="7"/>
-      <c r="G23" s="7"/>
+      <c r="F23" s="6"/>
+      <c r="G23" s="6"/>
       <c r="H23" s="4"/>
     </row>
     <row r="24" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+      <c r="A24" s="16">
         <v>22</v>
       </c>
       <c r="B24" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="7" t="s">
+      <c r="C24" s="6" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="7" t="s">
+      <c r="D24" s="6" t="s">
         <v>119</v>
       </c>
       <c r="E24" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F24" s="7"/>
-      <c r="G24" s="7">
+      <c r="F24" s="6"/>
+      <c r="G24" s="6">
         <v>1987</v>
       </c>
       <c r="H24" s="4"/>
     </row>
     <row r="25" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+      <c r="A25" s="16">
         <v>23</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="C25" s="7" t="s">
+      <c r="C25" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="D25" s="7" t="s">
+      <c r="D25" s="6" t="s">
         <v>120</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7">
+      <c r="F25" s="6"/>
+      <c r="G25" s="6">
         <v>1994</v>
       </c>
       <c r="H25" s="4"/>
     </row>
     <row r="26" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+      <c r="A26" s="16">
         <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
+      <c r="C26" s="6"/>
+      <c r="D26" s="6"/>
       <c r="E26" s="4"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
       <c r="H26" s="4"/>
     </row>
     <row r="27" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+      <c r="A27" s="16">
         <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
+      <c r="C27" s="6"/>
+      <c r="D27" s="6"/>
       <c r="E27" s="4"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="6"/>
       <c r="H27" s="4"/>
     </row>
     <row r="28" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1617,7 +1689,7 @@
   <dimension ref="A1:Z31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1629,87 +1701,87 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
     </row>
     <row r="2" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="16" t="s">
         <v>43</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="16" t="s">
         <v>44</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="16" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+      <c r="A3" s="16">
         <v>1</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="7"/>
     </row>
     <row r="4" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+      <c r="A4" s="16">
         <v>2</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="7"/>
     </row>
     <row r="5" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+      <c r="A5" s="16">
         <v>3</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="7"/>
     </row>
     <row r="6" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="7" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1746,39 +1818,41 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:26" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
+      <c r="Y1" s="8"/>
+      <c r="Z1" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1787,24 +1861,145 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="13"/>
+    <col min="2" max="2" width="38.5703125" style="13" customWidth="1"/>
+    <col min="3" max="3" width="18.85546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" style="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.7109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>129</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+      <c r="AA1" s="15"/>
+    </row>
+    <row r="2" spans="1:27" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>139</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>132</v>
+      </c>
+      <c r="F2" s="18" t="s">
+        <v>133</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="J2" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="K2" s="18" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Z1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="13"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" s="1" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="15"/>
+      <c r="O1" s="15"/>
+      <c r="P1" s="15"/>
+      <c r="Q1" s="15"/>
+      <c r="R1" s="15"/>
+      <c r="S1" s="15"/>
+      <c r="T1" s="15"/>
+      <c r="U1" s="15"/>
+      <c r="V1" s="15"/>
+      <c r="W1" s="15"/>
+      <c r="X1" s="15"/>
+      <c r="Y1" s="15"/>
+      <c r="Z1" s="15"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
MainTEMPs - Slow progress: Rock Lobster Template - v05 ...
</commit_message>
<xml_diff>
--- a/Landings/LANDINGS_Rock_Lobster_(Jasus_lalandii).xlsx
+++ b/Landings/LANDINGS_Rock_Lobster_(Jasus_lalandii).xlsx
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="198">
   <si>
     <t>Index</t>
   </si>
@@ -628,10 +628,10 @@
     <t>Over-Catch FAR-NORTH</t>
   </si>
   <si>
-    <t>Quota FAR-NORTH (kg)</t>
+    <t xml:space="preserve">ZONES: </t>
   </si>
   <si>
-    <t xml:space="preserve">Units: </t>
+    <t>Quota FAR-NORTH</t>
   </si>
 </sst>
 </file>
@@ -1516,6 +1516,9 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1528,34 +1531,16 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="10" fillId="9" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="10" fillId="9" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="37" fontId="10" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="37" fontId="10" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="15" fontId="18" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1624,16 +1609,10 @@
     <xf numFmtId="0" fontId="15" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="37" fontId="10" fillId="9" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="10" fillId="9" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="37" fontId="10" fillId="9" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="10" fillId="9" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="37" fontId="10" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1642,13 +1621,34 @@
     <xf numFmtId="37" fontId="10" fillId="2" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="9" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="10" fillId="9" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="37" fontId="10" fillId="7" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="37" fontId="10" fillId="7" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="15" fontId="18" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1656,7 +1656,7 @@
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="21">
     <dxf>
       <fill>
         <patternFill>
@@ -1726,290 +1726,11 @@
       </fill>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
         <color theme="1"/>
       </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="8" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FFFFFF00"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="none">
           <bgColor auto="1"/>
@@ -2066,14 +1787,35 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
+          <bgColor theme="2" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="none">
-          <bgColor auto="1"/>
+        <patternFill>
+          <bgColor theme="2" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.14996795556505021"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="2" tint="-0.14996795556505021"/>
         </patternFill>
       </fill>
     </dxf>
@@ -10198,7 +9940,7 @@
     <sortCondition ref="B2:B31"/>
   </sortState>
   <conditionalFormatting sqref="A3:A300">
-    <cfRule type="notContainsBlanks" dxfId="42" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="20" priority="1">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18383,7 +18125,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A300">
-    <cfRule type="notContainsBlanks" dxfId="41" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="19" priority="1">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18401,8 +18143,8 @@
   <dimension ref="A1:AB301"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -18437,22 +18179,22 @@
       <c r="J1" s="4"/>
       <c r="K1" s="4"/>
       <c r="L1" s="4"/>
-      <c r="M1" s="168" t="s">
-        <v>197</v>
-      </c>
-      <c r="N1" s="168" t="s">
+      <c r="M1" s="127" t="s">
+        <v>196</v>
+      </c>
+      <c r="N1" s="127" t="s">
         <v>132</v>
       </c>
-      <c r="O1" s="168" t="s">
+      <c r="O1" s="127" t="s">
         <v>166</v>
       </c>
-      <c r="P1" s="168" t="s">
+      <c r="P1" s="127" t="s">
         <v>168</v>
       </c>
-      <c r="Q1" s="168" t="s">
+      <c r="Q1" s="127" t="s">
         <v>169</v>
       </c>
-      <c r="R1" s="168" t="s">
+      <c r="R1" s="127" t="s">
         <v>167</v>
       </c>
       <c r="S1" s="4"/>
@@ -18501,12 +18243,8 @@
       <c r="L2" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="M2" s="65" t="s">
-        <v>132</v>
-      </c>
-      <c r="N2" s="111" t="s">
-        <v>166</v>
-      </c>
+      <c r="M2" s="65"/>
+      <c r="N2" s="111"/>
       <c r="O2" s="111"/>
       <c r="P2" s="111"/>
       <c r="Q2" s="111"/>
@@ -30682,7 +30420,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3:A300">
-    <cfRule type="notContainsBlanks" dxfId="40" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="18" priority="1">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -30693,6 +30431,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:AB301"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -30734,12 +30475,12 @@
       <c r="G1" s="50" t="s">
         <v>146</v>
       </c>
-      <c r="H1" s="127" t="s">
+      <c r="H1" s="128" t="s">
         <v>147</v>
       </c>
-      <c r="I1" s="128"/>
-      <c r="J1" s="128"/>
-      <c r="K1" s="129"/>
+      <c r="I1" s="129"/>
+      <c r="J1" s="129"/>
+      <c r="K1" s="130"/>
       <c r="L1" s="24"/>
       <c r="M1" s="24"/>
       <c r="N1" s="24"/>
@@ -39191,7 +38932,7 @@
     <mergeCell ref="H1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:A300">
-    <cfRule type="notContainsBlanks" dxfId="39" priority="2">
+    <cfRule type="notContainsBlanks" dxfId="17" priority="2">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39209,11 +38950,14 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:AA820"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H4" sqref="H4"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -39307,10 +39051,11 @@
         <v>Far-North</v>
       </c>
       <c r="G3" s="67">
-        <v>28</v>
+        <v>3</v>
       </c>
       <c r="H3" s="67">
-        <v>2500</v>
+        <f>G3*65</f>
+        <v>195</v>
       </c>
       <c r="I3" s="3"/>
     </row>
@@ -50754,7 +50499,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A3">
-    <cfRule type="notContainsBlanks" dxfId="38" priority="1">
+    <cfRule type="notContainsBlanks" dxfId="16" priority="1">
       <formula>LEN(TRIM(A3))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -50790,7 +50535,7 @@
   <dimension ref="A1:Z281"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="M6" sqref="M6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -50836,22 +50581,22 @@
     </row>
     <row r="2" spans="1:26" s="7" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="124"/>
-      <c r="B2" s="152" t="str">
+      <c r="B2" s="147" t="str">
         <f>"Rock Lobster Season:  " &amp; '11. Quotas'!$D$1 &amp; "/" &amp; RIGHT('11. Quotas'!$D$1+1, 2)</f>
         <v>Rock Lobster Season:  2024/25</v>
       </c>
-      <c r="C2" s="153"/>
-      <c r="D2" s="154"/>
+      <c r="C2" s="148"/>
+      <c r="D2" s="149"/>
       <c r="E2" s="122"/>
-      <c r="F2" s="134" t="s">
+      <c r="F2" s="165" t="s">
         <v>191</v>
       </c>
-      <c r="G2" s="135"/>
+      <c r="G2" s="166"/>
       <c r="H2" s="124"/>
-      <c r="I2" s="164" t="s">
-        <v>196</v>
-      </c>
-      <c r="J2" s="165"/>
+      <c r="I2" s="133" t="s">
+        <v>197</v>
+      </c>
+      <c r="J2" s="134"/>
       <c r="K2" s="124"/>
       <c r="L2" s="124"/>
       <c r="M2" s="124"/>
@@ -50871,24 +50616,24 @@
     </row>
     <row r="3" spans="1:26" s="7" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="124"/>
-      <c r="B3" s="155" t="str">
+      <c r="B3" s="150" t="str">
         <f>"   ( 1 Nov " &amp; '11. Quotas'!$D$1 &amp; " - 30 Apr " &amp; '11. Quotas'!$D$1+1 &amp; " )"</f>
         <v xml:space="preserve">   ( 1 Nov 2024 - 30 Apr 2025 )</v>
       </c>
-      <c r="C3" s="156"/>
-      <c r="D3" s="157"/>
+      <c r="C3" s="151"/>
+      <c r="D3" s="152"/>
       <c r="E3" s="122"/>
-      <c r="F3" s="136" t="str">
+      <c r="F3" s="167" t="str">
         <f>IF(TEXT(MAX('12. Landings'!$B$3:$B$820), "dd MMMM yyyy")="00 January 1900", "No DATE Data FOUND !!!", TEXT(MAX('12. Landings'!$B$3:$B$820), "dd MMMM yyyy"))</f>
         <v>25 February 2024</v>
       </c>
-      <c r="G3" s="137"/>
+      <c r="G3" s="168"/>
       <c r="H3" s="124"/>
-      <c r="I3" s="162">
-        <f>IF($F$6=0, " - - - ", IF($F$6=" - - - ", " - - - ", VLOOKUP($B$6, '11. Quotas'!$B$3:$G$300, 3, FALSE)))</f>
-        <v>250</v>
-      </c>
-      <c r="J3" s="163"/>
+      <c r="I3" s="131" t="str">
+        <f>IF($F$6=0, " - - - ", IF($F$6=" - - - ", " - - - ", ROUND(VLOOKUP($B$6, '11. Quotas'!$B$3:$G$300, 3, FALSE), 0))) &amp; " kg   ( " &amp; (ROUND(VLOOKUP($B$6, '11. Quotas'!$B$3:$G$300, 3, FALSE), 0)/$F$6)*100 &amp; " % )"</f>
+        <v>250 kg   ( 6.25 % )</v>
+      </c>
+      <c r="J3" s="132"/>
       <c r="K3" s="124"/>
       <c r="L3" s="124"/>
       <c r="M3" s="124"/>
@@ -50936,21 +50681,21 @@
     </row>
     <row r="5" spans="1:26" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="122"/>
-      <c r="B5" s="140" t="s">
+      <c r="B5" s="135" t="s">
         <v>186</v>
       </c>
-      <c r="C5" s="141"/>
-      <c r="D5" s="142"/>
+      <c r="C5" s="136"/>
+      <c r="D5" s="137"/>
       <c r="E5" s="122"/>
-      <c r="F5" s="158" t="s">
+      <c r="F5" s="153" t="s">
         <v>188</v>
       </c>
-      <c r="G5" s="159"/>
+      <c r="G5" s="154"/>
       <c r="H5" s="122"/>
-      <c r="I5" s="164" t="s">
+      <c r="I5" s="133" t="s">
         <v>193</v>
       </c>
-      <c r="J5" s="165"/>
+      <c r="J5" s="134"/>
       <c r="K5" s="122"/>
       <c r="L5" s="122"/>
       <c r="M5" s="122"/>
@@ -50970,23 +50715,23 @@
     </row>
     <row r="6" spans="1:26" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="122"/>
-      <c r="B6" s="143" t="s">
+      <c r="B6" s="138" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="144"/>
-      <c r="D6" s="145"/>
+      <c r="C6" s="139"/>
+      <c r="D6" s="140"/>
       <c r="E6" s="122"/>
-      <c r="F6" s="169">
+      <c r="F6" s="157">
         <f>IF($B$6="", " - - - ", _xlfn.IFNA(VLOOKUP($B$6, '11. Quotas'!$B$3:$G$300, 2, FALSE), " - - - "))</f>
         <v>4000</v>
       </c>
-      <c r="G6" s="170"/>
+      <c r="G6" s="158"/>
       <c r="H6" s="122"/>
-      <c r="I6" s="162" t="str">
+      <c r="I6" s="131" t="str">
         <f>IF($F$6=0, " - - - ", IF($F$6=" - - - ", " - - - ", TEXT(SUMIFS('12. Landings'!$H$3:$H$820, '12. Landings'!$C$3:$C$820, '22. RH Stats'!$B$6, '12. Landings'!$F$3:$F$820, '02. META-Areas'!$N$1), "#,##0"))&amp; " kg")</f>
-        <v>2,500 kg</v>
-      </c>
-      <c r="J6" s="163"/>
+        <v>195 kg</v>
+      </c>
+      <c r="J6" s="132"/>
       <c r="K6" s="122"/>
       <c r="L6" s="122"/>
       <c r="M6" s="122"/>
@@ -51006,9 +50751,9 @@
     </row>
     <row r="7" spans="1:26" ht="5.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="122"/>
-      <c r="B7" s="146"/>
-      <c r="C7" s="147"/>
-      <c r="D7" s="148"/>
+      <c r="B7" s="141"/>
+      <c r="C7" s="142"/>
+      <c r="D7" s="143"/>
       <c r="E7" s="122"/>
       <c r="F7" s="122"/>
       <c r="G7" s="122"/>
@@ -51034,19 +50779,19 @@
     </row>
     <row r="8" spans="1:26" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="122"/>
-      <c r="B8" s="146"/>
-      <c r="C8" s="147"/>
-      <c r="D8" s="148"/>
+      <c r="B8" s="141"/>
+      <c r="C8" s="142"/>
+      <c r="D8" s="143"/>
       <c r="E8" s="122"/>
-      <c r="F8" s="160" t="s">
+      <c r="F8" s="155" t="s">
         <v>190</v>
       </c>
-      <c r="G8" s="161"/>
+      <c r="G8" s="156"/>
       <c r="H8" s="122"/>
-      <c r="I8" s="164" t="s">
+      <c r="I8" s="133" t="s">
         <v>194</v>
       </c>
-      <c r="J8" s="165"/>
+      <c r="J8" s="134"/>
       <c r="K8" s="122"/>
       <c r="L8" s="122"/>
       <c r="M8" s="122"/>
@@ -51066,18 +50811,21 @@
     </row>
     <row r="9" spans="1:26" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="122"/>
-      <c r="B9" s="149"/>
-      <c r="C9" s="150"/>
-      <c r="D9" s="151"/>
+      <c r="B9" s="144"/>
+      <c r="C9" s="145"/>
+      <c r="D9" s="146"/>
       <c r="E9" s="122"/>
-      <c r="F9" s="162">
+      <c r="F9" s="131">
         <f>IF($F$6=0, " - - - ", IF($F$6=" - - - ", " - - - ", SUMIFS('12. Landings'!$H$3:$H$820, '12. Landings'!$C$3:$C$820, '22. RH Stats'!$B$6)))</f>
-        <v>2500</v>
-      </c>
-      <c r="G9" s="163"/>
+        <v>195</v>
+      </c>
+      <c r="G9" s="132"/>
       <c r="H9" s="122"/>
-      <c r="I9" s="162"/>
-      <c r="J9" s="163"/>
+      <c r="I9" s="131" t="str">
+        <f>IF($F$6=0, " - - - ", IF($F$6=" - - - ", " - - - ", ROUND(VLOOKUP($B$6, '11. Quotas'!$B$3:$G$300, 3, FALSE), 0))) - SUMIFS('12. Landings'!$H$3:$H$820, '12. Landings'!$C$3:$C$820, '22. RH Stats'!$B$6, '12. Landings'!$F$3:$F$820, '02. META-Areas'!$N$1) &amp; " kg"</f>
+        <v>55 kg</v>
+      </c>
+      <c r="J9" s="132"/>
       <c r="K9" s="122"/>
       <c r="L9" s="122"/>
       <c r="M9" s="122"/>
@@ -51129,10 +50877,10 @@
       <c r="C11" s="122"/>
       <c r="D11" s="122"/>
       <c r="E11" s="122"/>
-      <c r="F11" s="130" t="s">
+      <c r="F11" s="161" t="s">
         <v>189</v>
       </c>
-      <c r="G11" s="131"/>
+      <c r="G11" s="162"/>
       <c r="H11" s="122"/>
       <c r="I11" s="122"/>
       <c r="J11" s="122"/>
@@ -51159,11 +50907,11 @@
       <c r="C12" s="122"/>
       <c r="D12" s="122"/>
       <c r="E12" s="122"/>
-      <c r="F12" s="132" t="str">
+      <c r="F12" s="163" t="str">
         <f>IF($F$6=" - - - ", " - - - ", IF($F$6=0, " - - - ", IF((F9/F6)*100&gt;99, ROUND((F9/F6)*100, 0), IF((F9/F6)*100&gt;10,ROUND((F9/F6)*100, 1), ROUND((F9/F6)*100, 2))) &amp; " %"))</f>
-        <v>62.5 %</v>
-      </c>
-      <c r="G12" s="133"/>
+        <v>4.88 %</v>
+      </c>
+      <c r="G12" s="164"/>
       <c r="H12" s="122"/>
       <c r="I12" s="122"/>
       <c r="J12" s="122"/>
@@ -51218,15 +50966,15 @@
       <c r="C14" s="122"/>
       <c r="D14" s="122"/>
       <c r="E14" s="122"/>
-      <c r="F14" s="138" t="s">
+      <c r="F14" s="169" t="s">
         <v>192</v>
       </c>
-      <c r="G14" s="139"/>
+      <c r="G14" s="170"/>
       <c r="H14" s="122"/>
-      <c r="I14" s="164" t="s">
+      <c r="I14" s="133" t="s">
         <v>195</v>
       </c>
-      <c r="J14" s="165"/>
+      <c r="J14" s="134"/>
       <c r="K14" s="122"/>
       <c r="L14" s="122"/>
       <c r="M14" s="122"/>
@@ -51250,14 +50998,14 @@
       <c r="C15" s="122"/>
       <c r="D15" s="122"/>
       <c r="E15" s="122"/>
-      <c r="F15" s="166" t="str">
+      <c r="F15" s="159" t="str">
         <f>IF($F$6=" - - - ", " - - - ", IF($F$6=0, " - - - ", IF($F$9&gt;$F$6, IF((($F$9-$F$6)/$F$6)*100&gt;99, ROUND((($F$9-$F$6)/$F$6)*100, 0), IF((($F$9-$F$6)/$F$6)*100&gt;10,ROUND((($F$9-$F$6)/$F$6)*100, 1), ROUND((($F$9-$F$6)/$F$6)*100, 2))) &amp; " %", "0.00 %")))</f>
         <v>0.00 %</v>
       </c>
-      <c r="G15" s="167"/>
+      <c r="G15" s="160"/>
       <c r="H15" s="122"/>
-      <c r="I15" s="162"/>
-      <c r="J15" s="163"/>
+      <c r="I15" s="131"/>
+      <c r="J15" s="132"/>
       <c r="K15" s="122"/>
       <c r="L15" s="122"/>
       <c r="M15" s="122"/>
@@ -58725,11 +58473,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="I9:J9"/>
-    <mergeCell ref="I14:J14"/>
-    <mergeCell ref="I15:J15"/>
-    <mergeCell ref="I5:J5"/>
-    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="F15:G15"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="F14:G14"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="I8:J8"/>
@@ -58741,21 +58490,20 @@
     <mergeCell ref="F8:G8"/>
     <mergeCell ref="F6:G6"/>
     <mergeCell ref="F9:G9"/>
-    <mergeCell ref="F15:G15"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="F14:G14"/>
+    <mergeCell ref="I9:J9"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I5:J5"/>
+    <mergeCell ref="I6:J6"/>
   </mergeCells>
   <conditionalFormatting sqref="F6:G6">
     <cfRule type="cellIs" priority="22" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="23" operator="equal">
       <formula>" - - - "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="24" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58763,10 +58511,10 @@
     <cfRule type="cellIs" priority="19" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="20" operator="equal">
       <formula>" - - - "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="21" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58774,10 +58522,10 @@
     <cfRule type="cellIs" priority="16" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="17" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="17" operator="equal">
       <formula>" - - - "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="10" priority="18" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58785,10 +58533,10 @@
     <cfRule type="cellIs" priority="13" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="14" operator="equal">
       <formula>" - - - "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="8" priority="15" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58796,10 +58544,10 @@
     <cfRule type="cellIs" priority="10" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="equal">
       <formula>" - - - "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58807,10 +58555,10 @@
     <cfRule type="cellIs" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="8" operator="equal">
       <formula>" - - - "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="4" priority="9" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58818,10 +58566,10 @@
     <cfRule type="cellIs" priority="4" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="equal">
       <formula>" - - - "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -58829,14 +58577,14 @@
     <cfRule type="cellIs" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>" - - - "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThanOrEqual">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" sqref="B6:D9">
       <formula1>DDList_META_SRL_RightHolders</formula1>
     </dataValidation>

</xml_diff>